<commit_message>
Fixed logging. Added new benchmark code.
</commit_message>
<xml_diff>
--- a/snorocket-benchmark/src/site/resources/benchmark_december_webinar.xlsx
+++ b/snorocket-benchmark/src/site/resources/benchmark_december_webinar.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="benchmark_december_webinar" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -124,18 +124,6 @@
     <t>2012-12-19T13_52_42</t>
   </si>
   <si>
-    <t>Axiom Transformation Time</t>
-  </si>
-  <si>
-    <t>Axiom Loading Time</t>
-  </si>
-  <si>
-    <t>Classification Time</t>
-  </si>
-  <si>
-    <t>Taxonomy Construction Time</t>
-  </si>
-  <si>
     <t>Total Time</t>
   </si>
   <si>
@@ -221,6 +209,18 @@
   </si>
   <si>
     <t>2012-12-20T08_42_02</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Loading</t>
+  </si>
+  <si>
+    <t>Indexing</t>
+  </si>
+  <si>
+    <t>Taxonomy</t>
   </si>
 </sst>
 </file>
@@ -761,26 +761,19 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-AU"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>Classification Time</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1034966644113446"/>
+          <c:y val="8.4281208270018892E-2"/>
+          <c:w val="0.86607662211588432"/>
+          <c:h val="0.78391260302988441"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -796,16 +789,16 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Axiom Transformation Time</c:v>
+                  <c:v>Loading</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Axiom Loading Time</c:v>
+                  <c:v>Indexing</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Classification Time</c:v>
+                  <c:v>Classification</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Taxonomy Construction Time</c:v>
+                  <c:v>Taxonomy</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Total Time</c:v>
@@ -820,10 +813,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>19278.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1982.9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19278.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10722.6</c:v>
@@ -851,10 +844,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>17503.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2921.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17503.400000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22151.200000000001</c:v>
@@ -869,26 +862,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="49248896"/>
-        <c:axId val="61937152"/>
+        <c:axId val="54618368"/>
+        <c:axId val="56254464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49248896"/>
+        <c:axId val="54618368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61937152"/>
+        <c:crossAx val="56254464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61937152"/>
+        <c:axId val="56254464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,20 +912,39 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49248896"/>
+        <c:crossAx val="54618368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11942799802577604"/>
+          <c:y val="0.14086401965711737"/>
+          <c:w val="0.21141467528265068"/>
+          <c:h val="0.10259809013235048"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1024,26 +1035,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="107087360"/>
-        <c:axId val="107102208"/>
+        <c:axId val="56174080"/>
+        <c:axId val="56175616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107087360"/>
+        <c:axId val="56174080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107102208"/>
+        <c:crossAx val="56175616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107102208"/>
+        <c:axId val="56175616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1070,7 +1080,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107087360"/>
+        <c:crossAx val="56174080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1083,7 +1093,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1334,11 +1344,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="107094400"/>
-        <c:axId val="107095936"/>
+        <c:axId val="56206080"/>
+        <c:axId val="56208000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107094400"/>
+        <c:axId val="56206080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,14 +1373,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107095936"/>
+        <c:crossAx val="56208000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107095936"/>
+        <c:axId val="56208000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1396,7 +1406,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107094400"/>
+        <c:crossAx val="56206080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1409,7 +1419,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1421,8 +1431,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
@@ -1797,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1830,19 +1840,19 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
@@ -1865,10 +1875,10 @@
         <v>14</v>
       </c>
       <c r="E2">
+        <v>21012</v>
+      </c>
+      <c r="F2">
         <v>2961</v>
-      </c>
-      <c r="F2">
-        <v>21012</v>
       </c>
       <c r="G2">
         <v>12614</v>
@@ -1900,10 +1910,10 @@
         <v>14</v>
       </c>
       <c r="E3">
+        <v>19555</v>
+      </c>
+      <c r="F3">
         <v>2779</v>
-      </c>
-      <c r="F3">
-        <v>19555</v>
       </c>
       <c r="G3">
         <v>11849</v>
@@ -1935,10 +1945,10 @@
         <v>14</v>
       </c>
       <c r="E4">
+        <v>19074</v>
+      </c>
+      <c r="F4">
         <v>1753</v>
-      </c>
-      <c r="F4">
-        <v>19074</v>
       </c>
       <c r="G4">
         <v>10272</v>
@@ -1970,10 +1980,10 @@
         <v>14</v>
       </c>
       <c r="E5">
+        <v>19020</v>
+      </c>
+      <c r="F5">
         <v>1765</v>
-      </c>
-      <c r="F5">
-        <v>19020</v>
       </c>
       <c r="G5">
         <v>10677</v>
@@ -2005,10 +2015,10 @@
         <v>14</v>
       </c>
       <c r="E6">
+        <v>19346</v>
+      </c>
+      <c r="F6">
         <v>1780</v>
-      </c>
-      <c r="F6">
-        <v>19346</v>
       </c>
       <c r="G6">
         <v>10481</v>
@@ -2040,10 +2050,10 @@
         <v>14</v>
       </c>
       <c r="E7">
+        <v>19051</v>
+      </c>
+      <c r="F7">
         <v>1735</v>
-      </c>
-      <c r="F7">
-        <v>19051</v>
       </c>
       <c r="G7">
         <v>10330</v>
@@ -2075,10 +2085,10 @@
         <v>14</v>
       </c>
       <c r="E8">
+        <v>18899</v>
+      </c>
+      <c r="F8">
         <v>1780</v>
-      </c>
-      <c r="F8">
-        <v>18899</v>
       </c>
       <c r="G8">
         <v>9923</v>
@@ -2110,10 +2120,10 @@
         <v>14</v>
       </c>
       <c r="E9">
+        <v>18945</v>
+      </c>
+      <c r="F9">
         <v>1733</v>
-      </c>
-      <c r="F9">
-        <v>18945</v>
       </c>
       <c r="G9">
         <v>10368</v>
@@ -2145,10 +2155,10 @@
         <v>14</v>
       </c>
       <c r="E10">
+        <v>18996</v>
+      </c>
+      <c r="F10">
         <v>1748</v>
-      </c>
-      <c r="F10">
-        <v>18996</v>
       </c>
       <c r="G10">
         <v>10025</v>
@@ -2180,10 +2190,10 @@
         <v>14</v>
       </c>
       <c r="E11">
+        <v>18884</v>
+      </c>
+      <c r="F11">
         <v>1795</v>
-      </c>
-      <c r="F11">
-        <v>18884</v>
       </c>
       <c r="G11">
         <v>10687</v>
@@ -2203,31 +2213,31 @@
     </row>
     <row r="12" spans="1:11">
       <c r="E12">
-        <f>AVERAGE(E2:E11)</f>
-        <v>1982.9</v>
+        <f t="shared" ref="E12:K12" si="0">AVERAGE(E2:E11)</f>
+        <v>19278.2</v>
       </c>
       <c r="F12">
         <f>AVERAGE(F2:F11)</f>
-        <v>19278.2</v>
+        <v>1982.9</v>
       </c>
       <c r="G12">
-        <f>AVERAGE(G2:G11)</f>
+        <f t="shared" si="0"/>
         <v>10722.6</v>
       </c>
       <c r="H12">
-        <f>AVERAGE(H2:H11)</f>
+        <f t="shared" si="0"/>
         <v>2819.8</v>
       </c>
       <c r="I12">
-        <f>AVERAGE(I2:I11)</f>
+        <f t="shared" si="0"/>
         <v>34803.5</v>
       </c>
       <c r="J12">
-        <f>AVERAGE(J2:J11)</f>
+        <f t="shared" si="0"/>
         <v>2711469433.5999999</v>
       </c>
       <c r="K12">
-        <f>AVERAGE(K2:K11)</f>
+        <f t="shared" si="0"/>
         <v>4067963699.1999998</v>
       </c>
     </row>
@@ -2245,10 +2255,10 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
         <v>5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
@@ -2260,10 +2270,10 @@
         <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2280,10 +2290,10 @@
         <v>26</v>
       </c>
       <c r="E15">
+        <v>17939</v>
+      </c>
+      <c r="F15">
         <v>3834</v>
-      </c>
-      <c r="F15">
-        <v>17939</v>
       </c>
       <c r="G15">
         <v>23526</v>
@@ -2315,10 +2325,10 @@
         <v>26</v>
       </c>
       <c r="E16">
+        <v>17695</v>
+      </c>
+      <c r="F16">
         <v>3762</v>
-      </c>
-      <c r="F16">
-        <v>17695</v>
       </c>
       <c r="G16">
         <v>22556</v>
@@ -2350,10 +2360,10 @@
         <v>26</v>
       </c>
       <c r="E17">
+        <v>17482</v>
+      </c>
+      <c r="F17">
         <v>3092</v>
-      </c>
-      <c r="F17">
-        <v>17482</v>
       </c>
       <c r="G17">
         <v>21743</v>
@@ -2385,10 +2395,10 @@
         <v>26</v>
       </c>
       <c r="E18">
+        <v>17407</v>
+      </c>
+      <c r="F18">
         <v>3524</v>
-      </c>
-      <c r="F18">
-        <v>17407</v>
       </c>
       <c r="G18">
         <v>21920</v>
@@ -2420,10 +2430,10 @@
         <v>26</v>
       </c>
       <c r="E19">
+        <v>17371</v>
+      </c>
+      <c r="F19">
         <v>2511</v>
-      </c>
-      <c r="F19">
-        <v>17371</v>
       </c>
       <c r="G19">
         <v>21947</v>
@@ -2455,10 +2465,10 @@
         <v>26</v>
       </c>
       <c r="E20">
+        <v>17412</v>
+      </c>
+      <c r="F20">
         <v>2495</v>
-      </c>
-      <c r="F20">
-        <v>17412</v>
       </c>
       <c r="G20">
         <v>21837</v>
@@ -2490,10 +2500,10 @@
         <v>26</v>
       </c>
       <c r="E21">
+        <v>17494</v>
+      </c>
+      <c r="F21">
         <v>2497</v>
-      </c>
-      <c r="F21">
-        <v>17494</v>
       </c>
       <c r="G21">
         <v>22406</v>
@@ -2525,10 +2535,10 @@
         <v>26</v>
       </c>
       <c r="E22">
+        <v>17424</v>
+      </c>
+      <c r="F22">
         <v>2500</v>
-      </c>
-      <c r="F22">
-        <v>17424</v>
       </c>
       <c r="G22">
         <v>21837</v>
@@ -2560,10 +2570,10 @@
         <v>26</v>
       </c>
       <c r="E23">
+        <v>17423</v>
+      </c>
+      <c r="F23">
         <v>2495</v>
-      </c>
-      <c r="F23">
-        <v>17423</v>
       </c>
       <c r="G23">
         <v>22211</v>
@@ -2595,10 +2605,10 @@
         <v>26</v>
       </c>
       <c r="E24">
+        <v>17387</v>
+      </c>
+      <c r="F24">
         <v>2504</v>
-      </c>
-      <c r="F24">
-        <v>17387</v>
       </c>
       <c r="G24">
         <v>21529</v>
@@ -2619,36 +2629,36 @@
     <row r="25" spans="1:11">
       <c r="E25">
         <f>AVERAGE(E15:E24)</f>
-        <v>2921.4</v>
+        <v>17503.400000000001</v>
       </c>
       <c r="F25">
         <f>AVERAGE(F15:F24)</f>
-        <v>17503.400000000001</v>
+        <v>2921.4</v>
       </c>
       <c r="G25">
-        <f>AVERAGE(G15:G24)</f>
+        <f t="shared" ref="G25:K25" si="1">AVERAGE(G15:G24)</f>
         <v>22151.200000000001</v>
       </c>
       <c r="H25">
-        <f>AVERAGE(H15:H24)</f>
+        <f t="shared" si="1"/>
         <v>2574.6999999999998</v>
       </c>
       <c r="I25">
-        <f>AVERAGE(I15:I24)</f>
+        <f t="shared" si="1"/>
         <v>45150.7</v>
       </c>
       <c r="J25">
-        <f>AVERAGE(J15:J24)</f>
+        <f t="shared" si="1"/>
         <v>1347162559.2</v>
       </c>
       <c r="K25">
-        <f>AVERAGE(K15:K24)</f>
+        <f t="shared" si="1"/>
         <v>3983271526.4000001</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -2689,12 +2699,12 @@
         <v>11</v>
       </c>
       <c r="M52" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -2736,7 +2746,7 @@
     </row>
     <row r="54" spans="1:13">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -2782,27 +2792,27 @@
         <v>0</v>
       </c>
       <c r="G55">
-        <f t="shared" ref="G55:L55" si="0">AVERAGE(G53:G54)</f>
+        <f t="shared" ref="G55:L55" si="2">AVERAGE(G53:G54)</f>
         <v>0</v>
       </c>
       <c r="H55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>375.5</v>
       </c>
       <c r="I55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="J55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>407.5</v>
       </c>
       <c r="K55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2332629600</v>
       </c>
       <c r="L55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4023484416</v>
       </c>
     </row>
@@ -2844,12 +2854,12 @@
         <v>11</v>
       </c>
       <c r="M56" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B57">
         <v>4</v>
@@ -2891,7 +2901,7 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -2937,27 +2947,27 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <f t="shared" ref="G59:L59" si="1">AVERAGE(G57:G58)</f>
+        <f t="shared" ref="G59:L59" si="3">AVERAGE(G57:G58)</f>
         <v>0</v>
       </c>
       <c r="H59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>261.5</v>
       </c>
       <c r="I59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>33.5</v>
       </c>
       <c r="J59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>295</v>
       </c>
       <c r="K59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2972881136</v>
       </c>
       <c r="L59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4085481472</v>
       </c>
     </row>
@@ -2999,12 +3009,12 @@
         <v>11</v>
       </c>
       <c r="M60" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B61">
         <v>4</v>
@@ -3045,7 +3055,7 @@
     </row>
     <row r="62" spans="1:13">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -3090,27 +3100,27 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <f t="shared" ref="G63:L63" si="2">AVERAGE(G61:G62)</f>
+        <f t="shared" ref="G63:L63" si="4">AVERAGE(G61:G62)</f>
         <v>0</v>
       </c>
       <c r="H63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>207</v>
       </c>
       <c r="I63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="J63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>239</v>
       </c>
       <c r="K63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2788094176</v>
       </c>
       <c r="L63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4073914368</v>
       </c>
     </row>
@@ -3152,12 +3162,12 @@
         <v>11</v>
       </c>
       <c r="M64" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B65">
         <v>4</v>
@@ -3198,7 +3208,7 @@
     </row>
     <row r="66" spans="1:13">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B66">
         <v>4</v>
@@ -3243,27 +3253,27 @@
         <v>0.5</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:L67" si="3">AVERAGE(G65:G66)</f>
+        <f t="shared" ref="G67:L67" si="5">AVERAGE(G65:G66)</f>
         <v>0</v>
       </c>
       <c r="H67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1413.5</v>
       </c>
       <c r="I67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>149.5</v>
       </c>
       <c r="J67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1563.5</v>
       </c>
       <c r="K67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2277084640</v>
       </c>
       <c r="L67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4009328640</v>
       </c>
     </row>
@@ -3305,12 +3315,12 @@
         <v>11</v>
       </c>
       <c r="M68" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -3351,7 +3361,7 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -3396,27 +3406,27 @@
         <v>1</v>
       </c>
       <c r="G71">
-        <f t="shared" ref="G71:L71" si="4">AVERAGE(G69:G70)</f>
+        <f t="shared" ref="G71:L71" si="6">AVERAGE(G69:G70)</f>
         <v>0</v>
       </c>
       <c r="H71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1316</v>
       </c>
       <c r="I71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="J71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1378</v>
       </c>
       <c r="K71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2635709000</v>
       </c>
       <c r="L71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4034723840</v>
       </c>
     </row>
@@ -3458,12 +3468,12 @@
         <v>11</v>
       </c>
       <c r="M72" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B73">
         <v>4</v>
@@ -3505,7 +3515,7 @@
     </row>
     <row r="74" spans="1:13">
       <c r="A74" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B74">
         <v>4</v>
@@ -3551,27 +3561,27 @@
         <v>1</v>
       </c>
       <c r="G75">
-        <f t="shared" ref="G75:J75" si="5">AVERAGE(G73:G74)</f>
+        <f t="shared" ref="G75:J75" si="7">AVERAGE(G73:G74)</f>
         <v>0</v>
       </c>
       <c r="H75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1467.5</v>
       </c>
       <c r="I75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>69.5</v>
       </c>
       <c r="J75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1538</v>
       </c>
       <c r="K75">
-        <f t="shared" ref="K75" si="6">AVERAGE(K73:K74)</f>
+        <f t="shared" ref="K75" si="8">AVERAGE(K73:K74)</f>
         <v>2952471544</v>
       </c>
       <c r="L75">
-        <f t="shared" ref="L75" si="7">AVERAGE(L73:L74)</f>
+        <f t="shared" ref="L75" si="9">AVERAGE(L73:L74)</f>
         <v>4061986816</v>
       </c>
     </row>
@@ -3613,12 +3623,12 @@
         <v>11</v>
       </c>
       <c r="M76" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B77">
         <v>4</v>
@@ -3659,7 +3669,7 @@
     </row>
     <row r="78" spans="1:13">
       <c r="A78" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B78">
         <v>4</v>
@@ -3704,27 +3714,27 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <f t="shared" ref="G79:L79" si="8">AVERAGE(G77:G78)</f>
+        <f t="shared" ref="G79:L79" si="10">AVERAGE(G77:G78)</f>
         <v>0</v>
       </c>
       <c r="H79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2567.5</v>
       </c>
       <c r="I79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>288.5</v>
       </c>
       <c r="J79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2856</v>
       </c>
       <c r="K79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2643282924</v>
       </c>
       <c r="L79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4034625536</v>
       </c>
     </row>
@@ -3766,12 +3776,12 @@
         <v>11</v>
       </c>
       <c r="M80" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:13">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B81">
         <v>4</v>
@@ -3812,7 +3822,7 @@
     </row>
     <row r="82" spans="1:13">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -3857,27 +3867,27 @@
         <v>1</v>
       </c>
       <c r="G83">
-        <f t="shared" ref="G83:L83" si="9">AVERAGE(G81:G82)</f>
+        <f t="shared" ref="G83:L83" si="11">AVERAGE(G81:G82)</f>
         <v>0</v>
       </c>
       <c r="H83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3464</v>
       </c>
       <c r="I83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>446.5</v>
       </c>
       <c r="J83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3911.5</v>
       </c>
       <c r="K83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3045635636</v>
       </c>
       <c r="L83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4033544192</v>
       </c>
     </row>
@@ -3919,12 +3929,12 @@
         <v>11</v>
       </c>
       <c r="M84" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" spans="1:13">
       <c r="A85" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B85">
         <v>4</v>
@@ -3965,7 +3975,7 @@
     </row>
     <row r="86" spans="1:13">
       <c r="A86" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B86">
         <v>4</v>
@@ -4010,27 +4020,27 @@
         <v>1</v>
       </c>
       <c r="G87">
-        <f t="shared" ref="G87:L87" si="10">AVERAGE(G85:G86)</f>
+        <f t="shared" ref="G87:L87" si="12">AVERAGE(G85:G86)</f>
         <v>0</v>
       </c>
       <c r="H87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4491</v>
       </c>
       <c r="I87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>951</v>
       </c>
       <c r="J87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5443</v>
       </c>
       <c r="K87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2979681036</v>
       </c>
       <c r="L87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4078075904</v>
       </c>
     </row>
@@ -4072,12 +4082,12 @@
         <v>11</v>
       </c>
       <c r="M88" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="89" spans="1:13">
       <c r="A89" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B89">
         <v>4</v>
@@ -4118,7 +4128,7 @@
     </row>
     <row r="90" spans="1:13">
       <c r="A90" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B90">
         <v>4</v>
@@ -4163,27 +4173,27 @@
         <v>2</v>
       </c>
       <c r="G91">
-        <f t="shared" ref="G91:L91" si="11">AVERAGE(G89:G90)</f>
+        <f t="shared" ref="G91:L91" si="13">AVERAGE(G89:G90)</f>
         <v>0</v>
       </c>
       <c r="H91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8911</v>
       </c>
       <c r="I91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1424</v>
       </c>
       <c r="J91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>10337</v>
       </c>
       <c r="K91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2963028072</v>
       </c>
       <c r="L91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4073488384</v>
       </c>
     </row>
@@ -4225,12 +4235,12 @@
         <v>11</v>
       </c>
       <c r="M92" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4271,7 +4281,7 @@
     </row>
     <row r="94" spans="1:13">
       <c r="A94" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4316,27 +4326,27 @@
         <v>4</v>
       </c>
       <c r="G95">
-        <f t="shared" ref="G95:L95" si="12">AVERAGE(G93:G94)</f>
+        <f t="shared" ref="G95:L95" si="14">AVERAGE(G93:G94)</f>
         <v>0</v>
       </c>
       <c r="H95">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>19754</v>
       </c>
       <c r="I95">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3972.5</v>
       </c>
       <c r="J95">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>23730.5</v>
       </c>
       <c r="K95">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2909725776</v>
       </c>
       <c r="L95">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4130308096</v>
       </c>
     </row>
@@ -4378,12 +4388,12 @@
         <v>11</v>
       </c>
       <c r="M96" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B97">
         <v>4</v>
@@ -4425,7 +4435,7 @@
     </row>
     <row r="98" spans="1:13">
       <c r="A98" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B98">
         <v>4</v>
@@ -4471,27 +4481,27 @@
         <v>7.5</v>
       </c>
       <c r="G99">
-        <f t="shared" ref="G99:L99" si="13">AVERAGE(G97:G98)</f>
+        <f t="shared" ref="G99:L99" si="15">AVERAGE(G97:G98)</f>
         <v>0</v>
       </c>
       <c r="H99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>35008.5</v>
       </c>
       <c r="I99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>6271</v>
       </c>
       <c r="J99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>41287</v>
       </c>
       <c r="K99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3164636348</v>
       </c>
       <c r="L99">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4190797824</v>
       </c>
     </row>

</xml_diff>